<commit_message>
style: añade color a los campos
</commit_message>
<xml_diff>
--- a/cronograma_estudio_cloud_engineer.xlsx
+++ b/cronograma_estudio_cloud_engineer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Leopp\escuela\Cursos\Minsait\Associate Cloud Engineer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEBEF13C-1B4B-4827-BAC9-FAE98B79BCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37958B37-B7D7-4D6C-91CD-B8CA1CB1243A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,13 +180,104 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -216,11 +307,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,13 +634,13 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
@@ -557,201 +663,201 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>